<commit_message>
write parameter estimates to file for paper
</commit_message>
<xml_diff>
--- a/tidy-data/model-param-numbers.xlsx
+++ b/tidy-data/model-param-numbers.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avanderlinden/Desktop/ruminantSDSE/tidy-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2956F1D0-1EC7-4E41-AB45-E44467EDE46E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE339868-4877-3C4B-9337-46FE809F8314}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="600" windowWidth="23440" windowHeight="12240" xr2:uid="{01DF7CF8-C960-9F48-890D-82FE475ACB4D}"/>
+    <workbookView xWindow="200" yWindow="600" windowWidth="25400" windowHeight="14580" xr2:uid="{01DF7CF8-C960-9F48-890D-82FE475ACB4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D2" sqref="D2:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,20 +485,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="1">
         <v>2</v>
       </c>
       <c r="F2" s="1">
         <f>SUM(D2:E2)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -506,20 +506,20 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+      <c r="F3" s="1">
+        <f>SUM(D3:E3)</f>
         <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" ref="F3:F11" si="0">SUM(D3:E3)</f>
-        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -527,7 +527,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -536,11 +536,11 @@
         <v>3</v>
       </c>
       <c r="E4" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>SUM(D4:E4)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -548,7 +548,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -557,11 +557,11 @@
         <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F5" s="1">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>SUM(D5:E5)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -569,7 +569,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>9</v>
@@ -578,11 +578,11 @@
         <v>5</v>
       </c>
       <c r="E6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f>SUM(D6:E6)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="136" x14ac:dyDescent="0.2">
@@ -590,7 +590,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>9</v>
@@ -599,11 +599,11 @@
         <v>5</v>
       </c>
       <c r="E7" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>SUM(D7:E7)</f>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="68" x14ac:dyDescent="0.2">
@@ -623,7 +623,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="0"/>
+        <f>SUM(D8:E8)</f>
         <v>6</v>
       </c>
     </row>
@@ -644,7 +644,7 @@
         <v>5</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="0"/>
+        <f>SUM(D9:E9)</f>
         <v>10</v>
       </c>
     </row>
@@ -665,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="1">
-        <f t="shared" si="0"/>
+        <f>SUM(D10:E10)</f>
         <v>3</v>
       </c>
     </row>
@@ -686,11 +686,15 @@
         <v>2</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="0"/>
+        <f>SUM(D11:E11)</f>
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F11">
+    <sortCondition ref="A2:A11"/>
+    <sortCondition ref="B2:B11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>